<commit_message>
Add test JSON file, and delete data files
</commit_message>
<xml_diff>
--- a/snow_amounts.xlsx
+++ b/snow_amounts.xlsx
@@ -385,10 +385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,10 +444,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>43101</v>
+        <v>42810</v>
       </c>
       <c r="B5">
-        <v>2.8</v>
+        <v>0</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -455,10 +455,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>43102</v>
+        <v>43101</v>
       </c>
       <c r="B6">
-        <v>1.3</v>
+        <v>2.8</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -466,10 +466,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>43103</v>
+        <v>43102</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>1.3</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -477,10 +477,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>43104</v>
+        <v>43103</v>
       </c>
       <c r="B8">
-        <v>6.7</v>
+        <v>0</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -488,32 +488,32 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>43105</v>
+        <v>43104</v>
       </c>
       <c r="B9">
-        <v>7.9</v>
+        <v>6.7</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>43106</v>
+        <v>43105</v>
       </c>
       <c r="B10">
-        <v>4.7</v>
+        <v>7.9</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>43107</v>
+        <v>43106</v>
       </c>
       <c r="B11">
-        <v>0.1</v>
+        <v>4.7</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -521,10 +521,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>43108</v>
+        <v>43107</v>
       </c>
       <c r="B12">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -532,20 +532,31 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
+        <v>43108</v>
+      </c>
+      <c r="B13">
+        <v>0.6</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>43109</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>0.3</v>
       </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="C14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>